<commit_message>
Added dynamic erosion radius, depending on solver and size
</commit_message>
<xml_diff>
--- a/Setup/MazeDimensions_human.xlsx
+++ b/Setup/MazeDimensions_human.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tabea\PycharmProjects\AntsShapes\Setup_Dimensions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tabea\PycharmProjects\AntsShapes\Setup\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -56,12 +56,6 @@
     <t>6.34, 1.02</t>
   </si>
   <si>
-    <t>3.31, 1.33</t>
-  </si>
-  <si>
-    <t>3.31, 1.90</t>
-  </si>
-  <si>
     <t>21.75, 5.77</t>
   </si>
   <si>
@@ -71,24 +65,12 @@
     <t>13.25, 7.37</t>
   </si>
   <si>
-    <t>6.34, 2.18</t>
-  </si>
-  <si>
-    <t>2.25, 1.33</t>
-  </si>
-  <si>
     <t>6.24, 1.05</t>
   </si>
   <si>
     <t>6.24, 2.25</t>
   </si>
   <si>
-    <t>3.24, 1.34</t>
-  </si>
-  <si>
-    <t>3.24, 1.98</t>
-  </si>
-  <si>
     <t>2.22, 0.91</t>
   </si>
   <si>
@@ -98,15 +80,6 @@
     <t>10.66, 4.765</t>
   </si>
   <si>
-    <t>6.52, 2.66</t>
-  </si>
-  <si>
-    <t>6.52, 3.74</t>
-  </si>
-  <si>
-    <t>4.41, 2.19</t>
-  </si>
-  <si>
     <t>21.75, 9.51</t>
   </si>
   <si>
@@ -114,6 +87,33 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>3.31, 1.3</t>
+  </si>
+  <si>
+    <t>6.34, 2.15</t>
+  </si>
+  <si>
+    <t>3.24, 1.3</t>
+  </si>
+  <si>
+    <t>3.24, 2.00</t>
+  </si>
+  <si>
+    <t>3.31, 1.93</t>
+  </si>
+  <si>
+    <t>2.18, 0.91</t>
+  </si>
+  <si>
+    <t>4.36, 2.19</t>
+  </si>
+  <si>
+    <t>6.52, 2.63</t>
+  </si>
+  <si>
+    <t>6.52, 3.76</t>
   </si>
 </sst>
 </file>
@@ -443,13 +443,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -476,16 +484,16 @@
         <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="G2" s="1"/>
     </row>
@@ -494,19 +502,19 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="G3" s="1"/>
     </row>
@@ -515,19 +523,19 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G4" s="1"/>
     </row>
@@ -536,19 +544,19 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="F5" s="2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="G5" s="1"/>
     </row>

</xml_diff>